<commit_message>
A few new data points and corrected OST counts.
</commit_message>
<xml_diff>
--- a/results/h5perf.xlsx
+++ b/results/h5perf.xlsx
@@ -562,7 +562,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,8 +614,14 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -656,7 +662,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,6 +681,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -751,10 +758,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$12</c:f>
+              <c:f>Write!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -787,16 +794,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$C$2:$C$12</c:f>
+              <c:f>Write!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>540.66</c:v>
                 </c:pt>
@@ -829,6 +839,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>43173.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48840.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -851,10 +864,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$12</c:f>
+              <c:f>Write!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -887,16 +900,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$D$2:$D$12</c:f>
+              <c:f>Write!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>469.7</c:v>
                 </c:pt>
@@ -951,10 +967,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$12</c:f>
+              <c:f>Write!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -987,16 +1003,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$E$2:$E$12</c:f>
+              <c:f>Write!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="4">
                   <c:v>6520.03</c:v>
                 </c:pt>
@@ -1039,10 +1058,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$12</c:f>
+              <c:f>Write!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1075,16 +1094,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$F$2:$F$12</c:f>
+              <c:f>Write!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>529.97</c:v>
                 </c:pt>
@@ -1117,6 +1139,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44477.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51850.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,10 +1164,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$12</c:f>
+              <c:f>Write!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1175,16 +1200,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$G$2:$G$12</c:f>
+              <c:f>Write!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>482.3</c:v>
                 </c:pt>
@@ -1239,10 +1267,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$12</c:f>
+              <c:f>Write!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1275,16 +1303,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$H$2:$H$12</c:f>
+              <c:f>Write!$H$2:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="4">
                   <c:v>6709.79</c:v>
                 </c:pt>
@@ -1321,11 +1352,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184702080"/>
-        <c:axId val="184703616"/>
+        <c:axId val="185173504"/>
+        <c:axId val="185175040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184702080"/>
+        <c:axId val="185173504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1335,7 +1366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184703616"/>
+        <c:crossAx val="185175040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1343,7 +1374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184703616"/>
+        <c:axId val="185175040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184702080"/>
+        <c:crossAx val="185173504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1454,10 +1485,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$12</c:f>
+              <c:f>Read!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1490,16 +1521,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$C$2:$C$12</c:f>
+              <c:f>Read!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2441.8200000000002</c:v>
                 </c:pt>
@@ -1532,6 +1566,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>28203.439999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26381.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,10 +1591,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$12</c:f>
+              <c:f>Read!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1590,16 +1627,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$D$2:$D$12</c:f>
+              <c:f>Read!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2077.4699999999998</c:v>
                 </c:pt>
@@ -1654,10 +1694,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$12</c:f>
+              <c:f>Read!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1690,16 +1730,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$E$2:$E$12</c:f>
+              <c:f>Read!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="4">
                   <c:v>1345.35</c:v>
                 </c:pt>
@@ -1742,10 +1785,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$12</c:f>
+              <c:f>Read!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1778,16 +1821,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$F$2:$F$12</c:f>
+              <c:f>Read!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2443.54</c:v>
                 </c:pt>
@@ -1820,6 +1866,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>27275.72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27064.639999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1842,10 +1891,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$12</c:f>
+              <c:f>Read!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1878,16 +1927,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$G$2:$G$12</c:f>
+              <c:f>Read!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2053.9299999999998</c:v>
                 </c:pt>
@@ -1942,10 +1994,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$12</c:f>
+              <c:f>Read!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1978,16 +2030,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$H$2:$H$12</c:f>
+              <c:f>Read!$H$2:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="4">
                   <c:v>1390.82</c:v>
                 </c:pt>
@@ -2024,11 +2079,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184532352"/>
-        <c:axId val="184538240"/>
+        <c:axId val="185204736"/>
+        <c:axId val="185206272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184532352"/>
+        <c:axId val="185204736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2038,7 +2093,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184538240"/>
+        <c:crossAx val="185206272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2046,7 +2101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184538240"/>
+        <c:axId val="185206272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,7 +2131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184532352"/>
+        <c:crossAx val="185204736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2103,14 +2158,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>42860</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>23810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:colOff>280989</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2140,15 +2195,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>42861</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>52386</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2475,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,7 +2817,7 @@
         <v>1024</v>
       </c>
       <c r="B12">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3">
         <v>43173.8</v>
@@ -2782,6 +2837,24 @@
       <c r="H12" s="9">
         <v>30370.48</v>
       </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2048</v>
+      </c>
+      <c r="B13">
+        <v>160</v>
+      </c>
+      <c r="C13" s="9">
+        <v>48840.41</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9">
+        <v>51850.83</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2792,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,7 +3152,7 @@
         <v>1024</v>
       </c>
       <c r="B12">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3">
         <v>28203.439999999999</v>
@@ -3099,6 +3172,32 @@
       <c r="H12" s="9">
         <v>30193.87</v>
       </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2048</v>
+      </c>
+      <c r="B13">
+        <v>160</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26381.58</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9">
+        <v>27064.639999999999</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A few more datapoints
</commit_message>
<xml_diff>
--- a/results/h5perf.xlsx
+++ b/results/h5perf.xlsx
@@ -562,7 +562,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,18 +577,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -612,16 +600,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -658,30 +648,27 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -758,10 +745,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$13</c:f>
+              <c:f>Write!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -797,16 +784,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$C$2:$C$13</c:f>
+              <c:f>Write!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>540.66</c:v>
                 </c:pt>
@@ -842,6 +835,12 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>48840.41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59018.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60140.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,10 +863,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$13</c:f>
+              <c:f>Write!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -903,16 +902,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$D$2:$D$13</c:f>
+              <c:f>Write!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>469.7</c:v>
                 </c:pt>
@@ -967,10 +972,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$13</c:f>
+              <c:f>Write!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1006,16 +1011,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$E$2:$E$13</c:f>
+              <c:f>Write!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="4">
                   <c:v>6520.03</c:v>
                 </c:pt>
@@ -1058,10 +1069,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$13</c:f>
+              <c:f>Write!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1097,16 +1108,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$F$2:$F$13</c:f>
+              <c:f>Write!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>529.97</c:v>
                 </c:pt>
@@ -1142,6 +1159,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>51850.83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>53074</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1164,10 +1184,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$13</c:f>
+              <c:f>Write!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1203,16 +1223,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$G$2:$G$13</c:f>
+              <c:f>Write!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>482.3</c:v>
                 </c:pt>
@@ -1267,10 +1293,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Write!$A$2:$A$13</c:f>
+              <c:f>Write!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1306,16 +1332,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Write!$H$2:$H$13</c:f>
+              <c:f>Write!$H$2:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="4">
                   <c:v>6709.79</c:v>
                 </c:pt>
@@ -1352,11 +1384,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="185173504"/>
-        <c:axId val="185175040"/>
+        <c:axId val="199853568"/>
+        <c:axId val="199855104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="185173504"/>
+        <c:axId val="199853568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185175040"/>
+        <c:crossAx val="199855104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1374,7 +1406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185175040"/>
+        <c:axId val="199855104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185173504"/>
+        <c:crossAx val="199853568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1485,10 +1517,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$13</c:f>
+              <c:f>Read!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1524,16 +1556,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$C$2:$C$13</c:f>
+              <c:f>Read!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2441.8200000000002</c:v>
                 </c:pt>
@@ -1569,6 +1607,12 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>26381.58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32830.629999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32127.040000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,10 +1635,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$13</c:f>
+              <c:f>Read!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1630,16 +1674,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$D$2:$D$13</c:f>
+              <c:f>Read!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2077.4699999999998</c:v>
                 </c:pt>
@@ -1694,10 +1744,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$13</c:f>
+              <c:f>Read!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1733,16 +1783,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$E$2:$E$13</c:f>
+              <c:f>Read!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="4">
                   <c:v>1345.35</c:v>
                 </c:pt>
@@ -1785,10 +1841,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$13</c:f>
+              <c:f>Read!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1824,16 +1880,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$F$2:$F$13</c:f>
+              <c:f>Read!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2443.54</c:v>
                 </c:pt>
@@ -1869,6 +1931,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>27064.639999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32910.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1891,10 +1956,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$13</c:f>
+              <c:f>Read!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1930,16 +1995,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$G$2:$G$13</c:f>
+              <c:f>Read!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2053.9299999999998</c:v>
                 </c:pt>
@@ -1994,10 +2065,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Read!$A$2:$A$13</c:f>
+              <c:f>Read!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2033,16 +2104,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Read!$H$2:$H$13</c:f>
+              <c:f>Read!$H$2:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="4">
                   <c:v>1390.82</c:v>
                 </c:pt>
@@ -2079,11 +2156,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="185204736"/>
-        <c:axId val="185206272"/>
+        <c:axId val="199884800"/>
+        <c:axId val="199886336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="185204736"/>
+        <c:axId val="199884800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2093,7 +2170,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185206272"/>
+        <c:crossAx val="199886336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2101,7 +2178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185206272"/>
+        <c:axId val="199886336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185204736"/>
+        <c:crossAx val="199884800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2530,10 +2607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,28 +2624,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2579,19 +2656,20 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>540.66</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
         <v>469.7</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9">
         <v>529.97</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="9">
         <v>482.3</v>
       </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2600,19 +2678,20 @@
       <c r="B3">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>370.37</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="9">
         <v>860.26</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9">
         <v>490.8</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="9">
         <v>818.83</v>
       </c>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2621,19 +2700,20 @@
       <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="9">
         <v>1898.91</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="9">
         <v>1594.11</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>1927.87</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="9">
         <v>1591.28</v>
       </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2642,19 +2722,20 @@
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="9">
         <v>3873.19</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="9">
         <v>2311.41</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
         <v>3345.25</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="9">
         <v>2245.9299999999998</v>
       </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2663,22 +2744,22 @@
       <c r="B6">
         <v>24</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="9">
         <v>6852.2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="9">
         <v>765.43</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="8">
         <v>6520.03</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="9">
         <v>6192.01</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="9">
         <v>866.38</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="8">
         <v>6709.79</v>
       </c>
     </row>
@@ -2689,22 +2770,22 @@
       <c r="B7">
         <v>24</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>8829.9599999999991</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="9">
         <v>4100.2700000000004</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="8">
         <v>9296.24</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="9">
         <v>10544.7</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="9">
         <v>4204.26</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="8">
         <v>8822.3799999999992</v>
       </c>
     </row>
@@ -2715,22 +2796,22 @@
       <c r="B8">
         <v>24</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="9">
         <v>7364.78</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="9">
         <v>3697.61</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="8">
         <v>8456.42</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="9">
         <v>9841.41</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="9">
         <v>4034.35</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="8">
         <v>9171.26</v>
       </c>
     </row>
@@ -2741,22 +2822,22 @@
       <c r="B9">
         <v>72</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="9">
         <v>18931.759999999998</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="9">
         <v>4772.5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="8">
         <v>16424.04</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="9">
         <v>18633.240000000002</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="9">
         <v>4633.32</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="8">
         <v>17379.29</v>
       </c>
     </row>
@@ -2767,22 +2848,22 @@
       <c r="B10">
         <v>72</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="9">
         <v>24276.34</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="9">
         <v>4193.93</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="8">
         <v>20685.419999999998</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="9">
         <v>22983.37</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="8">
         <v>4220.75</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="8">
         <v>18587.91</v>
       </c>
     </row>
@@ -2793,22 +2874,22 @@
       <c r="B11">
         <v>72</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="9">
         <v>27953.24</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="9">
         <v>3921.01</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>25733.24</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="9">
         <v>24372.94</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="9">
         <v>-1</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>22777.16</v>
       </c>
     </row>
@@ -2819,22 +2900,22 @@
       <c r="B12">
         <v>160</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="8">
         <v>43173.8</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="9">
         <v>-1</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>30437.439999999999</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="8">
         <v>44477.25</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="9">
         <v>-1</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>30370.48</v>
       </c>
     </row>
@@ -2845,16 +2926,50 @@
       <c r="B13">
         <v>160</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>48840.41</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="9">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8">
         <v>51850.83</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4096</v>
+      </c>
+      <c r="B14">
+        <v>160</v>
+      </c>
+      <c r="C14" s="8">
+        <v>59018.9</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8">
+        <v>53074</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <v>160</v>
+      </c>
+      <c r="C15" s="8">
+        <v>60140.84</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2865,10 +2980,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,28 +2997,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2914,19 +3029,20 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>2441.8200000000002</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
         <v>2077.4699999999998</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9">
         <v>2443.54</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="9">
         <v>2053.9299999999998</v>
       </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2935,19 +3051,20 @@
       <c r="B3">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="9">
         <v>688.19</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="9">
         <v>2850.38</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9">
         <v>621.05999999999995</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="9">
         <v>697.03</v>
       </c>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2956,19 +3073,20 @@
       <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="9">
         <v>330.08</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="9">
         <v>4132.18</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>456.96</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="9">
         <v>1315.91</v>
       </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2977,19 +3095,20 @@
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="9">
         <v>1419.47</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="9">
         <v>5600.63</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
         <v>1494.46</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="9">
         <v>1765.45</v>
       </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2998,22 +3117,22 @@
       <c r="B6">
         <v>24</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="9">
         <v>1464.56</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="9">
         <v>2728.62</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="8">
         <v>1345.35</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="9">
         <v>1430.44</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="9">
         <v>2768.19</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="8">
         <v>1390.82</v>
       </c>
     </row>
@@ -3024,22 +3143,22 @@
       <c r="B7">
         <v>24</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>4524.59</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="9">
         <v>4682.96</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="8">
         <v>3498.81</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="9">
         <v>3225.49</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="9">
         <v>3414.57</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="8">
         <v>3275.17</v>
       </c>
     </row>
@@ -3050,22 +3169,22 @@
       <c r="B8">
         <v>24</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="9">
         <v>7734.27</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="9">
         <v>4032.17</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="8">
         <v>7454.82</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="9">
         <v>5971.39</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="9">
         <v>3507.68</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="8">
         <v>7059.35</v>
       </c>
     </row>
@@ -3076,22 +3195,22 @@
       <c r="B9">
         <v>72</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="9">
         <v>13206.18</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="9">
         <v>4476.99</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="8">
         <v>12791.71</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="9">
         <v>11303.13</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="9">
         <v>3902.51</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="8">
         <v>11682.53</v>
       </c>
     </row>
@@ -3102,22 +3221,22 @@
       <c r="B10">
         <v>72</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="9">
         <v>18179.919999999998</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="9">
         <v>4088.96</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="8">
         <v>16189.58</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="9">
         <v>17415.22</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="8">
         <v>3774.96</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="8">
         <v>16647.240000000002</v>
       </c>
     </row>
@@ -3128,22 +3247,22 @@
       <c r="B11">
         <v>72</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="9">
         <v>25112.9</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="9">
         <v>4035.38</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>24473.3</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="9">
         <v>24954.94</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="9">
         <v>-1</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>24746</v>
       </c>
     </row>
@@ -3154,22 +3273,22 @@
       <c r="B12">
         <v>160</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="8">
         <v>28203.439999999999</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="9">
         <v>-1</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>31474.41</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="8">
         <v>27275.72</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="9">
         <v>-1</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>30193.87</v>
       </c>
     </row>
@@ -3180,24 +3299,50 @@
       <c r="B13">
         <v>160</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="9">
         <v>26381.58</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="9">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8">
         <v>27064.639999999999</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="A14">
+        <v>4096</v>
+      </c>
+      <c r="B14">
+        <v>160</v>
+      </c>
+      <c r="C14" s="8">
+        <v>32830.629999999997</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8">
+        <v>32910.33</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <v>160</v>
+      </c>
+      <c r="C15" s="8">
+        <v>32127.040000000001</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3228,28 +3373,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3513,7 +3658,7 @@
       <c r="B13">
         <v>640</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>655360</v>
       </c>
       <c r="D13">
@@ -3522,7 +3667,7 @@
       <c r="E13">
         <v>5760</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <v>660485</v>
       </c>
       <c r="G13">
@@ -3536,7 +3681,7 @@
       <c r="B14">
         <v>640</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>655360</v>
       </c>
       <c r="D14">
@@ -3545,7 +3690,7 @@
       <c r="E14">
         <v>670</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <v>655395</v>
       </c>
       <c r="G14">
@@ -3582,7 +3727,7 @@
       <c r="B16">
         <v>1270</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>1310710</v>
       </c>
       <c r="D16">
@@ -3591,7 +3736,7 @@
       <c r="E16">
         <v>4530</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="4">
         <v>1313980</v>
       </c>
       <c r="G16">
@@ -6081,7 +6226,7 @@
       <c r="G124">
         <v>1048480</v>
       </c>
-      <c r="H124" s="8"/>
+      <c r="H124" s="6"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -6105,7 +6250,7 @@
       <c r="G125">
         <v>2096640</v>
       </c>
-      <c r="H125" s="8"/>
+      <c r="H125" s="6"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -6129,7 +6274,7 @@
       <c r="G126">
         <v>136366259712</v>
       </c>
-      <c r="H126" s="8"/>
+      <c r="H126" s="6"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -6153,7 +6298,7 @@
       <c r="G127">
         <v>137442098656</v>
       </c>
-      <c r="H127" s="8"/>
+      <c r="H127" s="6"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -6177,7 +6322,7 @@
       <c r="G128">
         <v>640</v>
       </c>
-      <c r="H128" s="8"/>
+      <c r="H128" s="6"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
@@ -6201,7 +6346,7 @@
       <c r="G129">
         <v>640</v>
       </c>
-      <c r="H129" s="8"/>
+      <c r="H129" s="6"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
@@ -6225,7 +6370,7 @@
       <c r="G130">
         <v>5</v>
       </c>
-      <c r="H130" s="8"/>
+      <c r="H130" s="6"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -6249,19 +6394,19 @@
       <c r="G131">
         <v>630</v>
       </c>
-      <c r="H131" s="8"/>
+      <c r="H131" s="6"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>132</v>
       </c>
-      <c r="B132" s="7">
+      <c r="B132" s="5">
         <v>1073741824</v>
       </c>
-      <c r="C132" s="6">
+      <c r="C132" s="4">
         <v>1048576</v>
       </c>
-      <c r="D132" s="7">
+      <c r="D132" s="5">
         <v>1073741824</v>
       </c>
       <c r="E132">
@@ -6273,7 +6418,7 @@
       <c r="G132">
         <v>512</v>
       </c>
-      <c r="H132" s="8"/>
+      <c r="H132" s="6"/>
       <c r="I132" t="s">
         <v>170</v>
       </c>
@@ -6291,16 +6436,16 @@
       <c r="D133">
         <v>0</v>
       </c>
-      <c r="E133" s="7">
+      <c r="E133" s="5">
         <v>1073741824</v>
       </c>
-      <c r="F133" s="6">
+      <c r="F133" s="4">
         <v>1048576</v>
       </c>
-      <c r="G133" s="7">
+      <c r="G133" s="5">
         <v>1073741824</v>
       </c>
-      <c r="H133" s="8"/>
+      <c r="H133" s="6"/>
       <c r="I133" t="s">
         <v>171</v>
       </c>
@@ -6327,7 +6472,7 @@
       <c r="G134">
         <v>87</v>
       </c>
-      <c r="H134" s="8"/>
+      <c r="H134" s="6"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -6351,19 +6496,19 @@
       <c r="G135">
         <v>328</v>
       </c>
-      <c r="H135" s="8"/>
+      <c r="H135" s="6"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
-      <c r="B136" s="7">
+      <c r="B136" s="5">
         <v>1280</v>
       </c>
-      <c r="C136" s="6">
+      <c r="C136" s="4">
         <v>1310720</v>
       </c>
-      <c r="D136" s="7">
+      <c r="D136" s="5">
         <v>2560</v>
       </c>
       <c r="E136">
@@ -6375,7 +6520,7 @@
       <c r="G136">
         <v>5120</v>
       </c>
-      <c r="H136" s="8"/>
+      <c r="H136" s="6"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -6390,16 +6535,16 @@
       <c r="D137">
         <v>0</v>
       </c>
-      <c r="E137" s="7">
+      <c r="E137" s="5">
         <v>1920</v>
       </c>
-      <c r="F137" s="6">
+      <c r="F137" s="4">
         <v>1311350</v>
       </c>
-      <c r="G137" s="7">
+      <c r="G137" s="5">
         <v>3840</v>
       </c>
-      <c r="H137" s="8"/>
+      <c r="H137" s="6"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -6423,7 +6568,7 @@
       <c r="G138">
         <v>1270</v>
       </c>
-      <c r="H138" s="8"/>
+      <c r="H138" s="6"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -6447,7 +6592,7 @@
       <c r="G139">
         <v>1240</v>
       </c>
-      <c r="H139" s="8"/>
+      <c r="H139" s="6"/>
     </row>
     <row r="140" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
@@ -6609,7 +6754,7 @@
       <c r="G146">
         <v>5.8202999999999998E-2</v>
       </c>
-      <c r="H146" s="8"/>
+      <c r="H146" s="6"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
@@ -6633,7 +6778,7 @@
       <c r="G147">
         <v>9.2852359999999994</v>
       </c>
-      <c r="H147" s="8"/>
+      <c r="H147" s="6"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
@@ -6657,7 +6802,7 @@
       <c r="G148">
         <v>7.5721999999999998E-2</v>
       </c>
-      <c r="H148" s="8"/>
+      <c r="H148" s="6"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
@@ -6681,7 +6826,7 @@
       <c r="G149">
         <v>109.08995299999999</v>
       </c>
-      <c r="H149" s="8"/>
+      <c r="H149" s="6"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
@@ -6705,7 +6850,7 @@
       <c r="G150">
         <v>109.063537</v>
       </c>
-      <c r="H150" s="8"/>
+      <c r="H150" s="6"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
@@ -6729,7 +6874,7 @@
       <c r="G151">
         <v>95.556219999999996</v>
       </c>
-      <c r="H151" s="8"/>
+      <c r="H151" s="6"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
@@ -6753,7 +6898,7 @@
       <c r="G152">
         <v>3983.540082</v>
       </c>
-      <c r="H152" s="8"/>
+      <c r="H152" s="6"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
@@ -6777,7 +6922,7 @@
       <c r="G153">
         <v>2902.708247</v>
       </c>
-      <c r="H153" s="8"/>
+      <c r="H153" s="6"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
@@ -6801,7 +6946,7 @@
       <c r="G154">
         <v>20.068511999999998</v>
       </c>
-      <c r="H154" s="8"/>
+      <c r="H154" s="6"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
@@ -6825,7 +6970,7 @@
       <c r="G155">
         <v>60.417712000000002</v>
       </c>
-      <c r="H155" s="8"/>
+      <c r="H155" s="6"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
@@ -6849,7 +6994,7 @@
       <c r="G156">
         <v>3983.6235040000001</v>
       </c>
-      <c r="H156" s="8"/>
+      <c r="H156" s="6"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
@@ -6873,7 +7018,7 @@
       <c r="G157">
         <v>2902.7696219999998</v>
       </c>
-      <c r="H157" s="8"/>
+      <c r="H157" s="6"/>
     </row>
     <row r="158" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">

</xml_diff>